<commit_message>
update run for georgia
</commit_message>
<xml_diff>
--- a/georgia/transformations/templates/calibrated/georgia/model_input_variables_georgia_ce_calibrated.xlsx
+++ b/georgia/transformations/templates/calibrated/georgia/model_input_variables_georgia_ce_calibrated.xlsx
@@ -8,9 +8,9 @@
   </bookViews>
   <sheets>
     <sheet name="strategy_id-0" sheetId="1" r:id="rId1"/>
-    <sheet name="strategy_id-6003" sheetId="2" r:id="rId2"/>
-    <sheet name="strategy_id-6004" sheetId="3" r:id="rId3"/>
-    <sheet name="strategy_id-6005" sheetId="4" r:id="rId4"/>
+    <sheet name="strategy_id-6004" sheetId="2" r:id="rId2"/>
+    <sheet name="strategy_id-6005" sheetId="3" r:id="rId3"/>
+    <sheet name="strategy_id-6006" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>